<commit_message>
Completed partial Project Report Template
</commit_message>
<xml_diff>
--- a/Excels/Project Schedule.xlsx
+++ b/Excels/Project Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Pendrive 1.0\University\Semester 10\Software Engineering\Lab\FINAL\GitArchieve\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE21C58-A2E3-41BB-BE6A-B4DD670B04EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFD445C-2496-4250-AC30-A3D62066061F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D0B47201-0EE1-4C4E-BF77-96B70980784A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D0B47201-0EE1-4C4E-BF77-96B70980784A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,146 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
-  <si>
-    <t>Splash Screen</t>
-  </si>
-  <si>
-    <t>Swipe Animation with Information with carousel effect for first time open</t>
-  </si>
-  <si>
-    <t>Login or signup</t>
-  </si>
-  <si>
-    <t>upload profile picture</t>
-  </si>
-  <si>
-    <t>User must fill up basic information</t>
-  </si>
-  <si>
-    <t>User need to allow the permission of location or manually select the co-ordinate of location from maps</t>
-  </si>
-  <si>
-    <t>Search bar with filtering option</t>
-  </si>
-  <si>
-    <t>Most popular hospital lists on carousel effect</t>
-  </si>
-  <si>
-    <t>Favorite items on carousel effect</t>
-  </si>
-  <si>
-    <t>List of all available services</t>
-  </si>
-  <si>
-    <t>Home Screen icon</t>
-  </si>
-  <si>
-    <t>Medicine Reminder icon</t>
-  </si>
-  <si>
-    <t>Blog Page Icon</t>
-  </si>
-  <si>
-    <t>AI Doctor</t>
-  </si>
-  <si>
-    <t>User profile page</t>
-  </si>
-  <si>
-    <t>Order History menu</t>
-  </si>
-  <si>
-    <t>Track Appointment</t>
-  </si>
-  <si>
-    <t>Active Orders (Booked Cabin, oxygen cylinder, ambulance etc.)</t>
-  </si>
-  <si>
-    <t>All the page that has been opened from another page, will be pushed to stack of history</t>
-  </si>
-  <si>
-    <t>Support mobile banking, card and pay cash by hand option (for limited services like appoinment)</t>
-  </si>
-  <si>
-    <t>Can comment and rating to doctor and hospital</t>
-  </si>
-  <si>
-    <t>Can read all the essential information of hospital and doctor like age, degrees, availability, location, gender, age, name, ratings, comments etc.</t>
-  </si>
-  <si>
-    <t>Can read history of everything</t>
-  </si>
-  <si>
-    <t>Can Create, read, update and delete accounts, credentials, reports.</t>
-  </si>
-  <si>
-    <t>Can create, read, update and delete new moderators</t>
-  </si>
-  <si>
-    <t>Can change username, password</t>
-  </si>
-  <si>
-    <t>Basic Information</t>
-  </si>
-  <si>
-    <t>Can see most recent comments with view all options</t>
-  </si>
-  <si>
-    <t>Can see list of serial appointed by patient with view all options</t>
-  </si>
-  <si>
-    <t>Welcome Page</t>
-  </si>
-  <si>
-    <t>Account Options</t>
-  </si>
-  <si>
-    <t>Reviews</t>
-  </si>
-  <si>
-    <t>Blog page</t>
-  </si>
-  <si>
-    <t>Can see and create read update and delete doctor lists</t>
-  </si>
-  <si>
-    <t>Can see the requested list of doctor queued for approve</t>
-  </si>
-  <si>
-    <t>Cabin section where all the cabin related things will maintains</t>
-  </si>
-  <si>
-    <t>All track list of equipents</t>
-  </si>
-  <si>
-    <t>Track list of ambulance</t>
-  </si>
-  <si>
-    <t>Section for handling users queries</t>
-  </si>
-  <si>
-    <t>Histoy of patient</t>
-  </si>
-  <si>
-    <t>Patient</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Hospital</t>
-  </si>
-  <si>
-    <t>Doctor</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
   <si>
     <t>Serial</t>
   </si>
   <si>
-    <t>Role</t>
-  </si>
-  <si>
     <t>Task Name</t>
   </si>
   <si>
@@ -225,6 +90,147 @@
   </si>
   <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>Identify stakeholders (patients, doctors, hospitals, admin)</t>
+  </si>
+  <si>
+    <t>Gather functional requirements (appointments, bed booking, AI chat)</t>
+  </si>
+  <si>
+    <t>Gather non-functional requirements (security, scalability, usability)</t>
+  </si>
+  <si>
+    <t>Define use cases and user roles</t>
+  </si>
+  <si>
+    <t>Review and validate requirements with stakeholders</t>
+  </si>
+  <si>
+    <t>Create initial product backlog in Trello</t>
+  </si>
+  <si>
+    <t>Define system architecture (client-server, APIs)</t>
+  </si>
+  <si>
+    <t>Create database schema (ER diagram)</t>
+  </si>
+  <si>
+    <t>Design UI/UX wireframes for patient/doctor/hospital apps</t>
+  </si>
+  <si>
+    <t>Define API endpoints and integration plan</t>
+  </si>
+  <si>
+    <t>Plan AI Doctor module architecture</t>
+  </si>
+  <si>
+    <t>Design admin panel structure with reporting tools</t>
+  </si>
+  <si>
+    <t>Review and finalize system design document</t>
+  </si>
+  <si>
+    <t>Develop user authentication (signup, login, JWT security)</t>
+  </si>
+  <si>
+    <t>Implement patient profile management</t>
+  </si>
+  <si>
+    <t>Implement doctor search and appointment booking</t>
+  </si>
+  <si>
+    <t>Develop hospital bed booking feature</t>
+  </si>
+  <si>
+    <t>Implement test ordering system</t>
+  </si>
+  <si>
+    <t>Develop patient–doctor chat interface</t>
+  </si>
+  <si>
+    <t>Integrate payment gateway (if applicable)</t>
+  </si>
+  <si>
+    <t>Review and test patient module features</t>
+  </si>
+  <si>
+    <t>Develop doctor profile management</t>
+  </si>
+  <si>
+    <t>Implement appointment scheduling and management</t>
+  </si>
+  <si>
+    <t>Create blog posting and review feature</t>
+  </si>
+  <si>
+    <t>Integrate chat with patients</t>
+  </si>
+  <si>
+    <t>Add hospital collaboration functionality</t>
+  </si>
+  <si>
+    <t>Review and test doctor module features</t>
+  </si>
+  <si>
+    <t>Implement hospital registration and profile management</t>
+  </si>
+  <si>
+    <t>CRUD for hospital equipment and test services</t>
+  </si>
+  <si>
+    <t>Manage patient requests (accept/reject system)</t>
+  </si>
+  <si>
+    <t>Develop hospital–doctor linking</t>
+  </si>
+  <si>
+    <t>Review and test hospital module features</t>
+  </si>
+  <si>
+    <t>Implement admin login and authentication</t>
+  </si>
+  <si>
+    <t>Manage users (patients, doctors, hospitals)</t>
+  </si>
+  <si>
+    <t>Add reporting &amp; graphs dashboard</t>
+  </si>
+  <si>
+    <t>Implement audit logs and monitoring</t>
+  </si>
+  <si>
+    <t>Develop symptom input form (NLP interface)</t>
+  </si>
+  <si>
+    <t>Train/integrate AI model for basic diagnosis suggestions</t>
+  </si>
+  <si>
+    <t>Test AI responses for accuracy &amp; safety</t>
+  </si>
+  <si>
+    <t>Unit testing for all modules</t>
+  </si>
+  <si>
+    <t>Integration testing (patient–doctor–hospital flow)</t>
+  </si>
+  <si>
+    <t>User Acceptance Testing (UAT) with stakeholders</t>
+  </si>
+  <si>
+    <t>Bug fixing and retesting</t>
+  </si>
+  <si>
+    <t>Deploy system to cloud/hosting server (CI/CD setup)</t>
+  </si>
+  <si>
+    <t>Publish app (mobile/web) and provide user documentation</t>
+  </si>
+  <si>
+    <t>Plan maintenance, updates, and future scalability</t>
+  </si>
+  <si>
+    <t>Prepare PRD</t>
   </si>
 </sst>
 </file>
@@ -232,7 +238,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -300,7 +306,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -637,60 +643,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C1AF02-3671-4699-A983-17717D3E4B01}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="B1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" customWidth="1"/>
-    <col min="4" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="9" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="66" customWidth="1"/>
+    <col min="4" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>44</v>
-      </c>
+    <row r="1" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1">
         <v>2</v>
@@ -700,19 +700,18 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1"/>
+    <row r="3" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -722,19 +721,18 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1"/>
+    <row r="4" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
       <c r="C4" s="3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -744,19 +742,18 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -766,26 +763,25 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1"/>
+    <row r="6" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1">
         <f>SUM(D2:D48)</f>
@@ -793,26 +789,25 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1"/>
+    <row r="7" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1">
         <v>3</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1">
         <f>SUM(D2:D27)</f>
@@ -820,26 +815,25 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="8" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F8" s="1">
         <v>3</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="I8" s="1">
         <f>SUM(D2:D22)</f>
@@ -847,26 +841,25 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="9" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1">
         <v>4</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="I9" s="1">
         <f>SUM(F2:F22)</f>
@@ -874,19 +867,18 @@
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="10" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1">
         <v>4</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -896,19 +888,18 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1">
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1">
         <v>3</v>
@@ -918,26 +909,25 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="12" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1">
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F12" s="1">
         <v>4</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="I12" s="1">
         <f>I8/I7</f>
@@ -945,26 +935,25 @@
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1">
         <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F13" s="1">
         <v>5</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="I13" s="1">
         <f>I8-I7</f>
@@ -972,26 +961,25 @@
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="14" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="I14" s="1">
         <f>I8/I9</f>
@@ -999,26 +987,25 @@
       </c>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F15" s="1">
         <v>4</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="I15" s="1">
         <f>I8-I9</f>
@@ -1026,19 +1013,18 @@
       </c>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="16" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1">
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F16" s="1">
         <v>3</v>
@@ -1048,77 +1034,74 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="17" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1">
         <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F17" s="1">
         <v>4</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="I17" s="6">
         <f>(I7/I6)*100</f>
         <v>53.521126760563376</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F18" s="1">
         <v>3</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="I18" s="6">
         <f>(I8/I6)*100</f>
         <v>42.95774647887324</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D19" s="1">
         <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F19" s="1">
         <v>4</v>
@@ -1128,19 +1111,18 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="20" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F20" s="1">
         <v>3</v>
@@ -1150,19 +1132,18 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="21" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
@@ -1172,19 +1153,18 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    <row r="22" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D22" s="1">
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F22" s="1">
         <v>4</v>
@@ -1194,19 +1174,18 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="23" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1">
         <v>4</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1214,21 +1193,18 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="24" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D24" s="1">
         <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1236,19 +1212,18 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+    <row r="25" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="1"/>
       <c r="C25" s="3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1">
         <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1256,19 +1231,18 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+    <row r="26" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="1"/>
       <c r="C26" s="3" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1276,19 +1250,18 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+    <row r="27" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="1"/>
       <c r="C27" s="3" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1">
         <v>3</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1296,21 +1269,18 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+    <row r="28" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D28" s="1">
         <v>4</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1318,19 +1288,18 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+    <row r="29" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D29" s="1">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1338,19 +1307,18 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+    <row r="30" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D30" s="1">
         <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1358,19 +1326,18 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+    <row r="31" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1"/>
       <c r="C31" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1378,19 +1345,18 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+    <row r="32" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="1"/>
       <c r="C32" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D32" s="1">
         <v>3</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1398,19 +1364,18 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+    <row r="33" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="1"/>
       <c r="C33" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D33" s="1">
         <v>4</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1418,19 +1383,18 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+    <row r="34" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="1"/>
       <c r="C34" s="2" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D34" s="1">
         <v>3</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -1438,19 +1402,18 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+    <row r="35" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="1"/>
       <c r="C35" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="D35" s="1">
         <v>3</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1458,19 +1421,18 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+    <row r="36" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="1"/>
       <c r="C36" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D36" s="1">
         <v>2</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -1478,19 +1440,18 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+    <row r="37" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="1"/>
       <c r="C37" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D37" s="1">
         <v>3</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1498,19 +1459,18 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+    <row r="38" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="1"/>
       <c r="C38" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D38" s="1">
         <v>4</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1518,19 +1478,18 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+    <row r="39" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="1"/>
       <c r="C39" s="2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D39" s="1">
         <v>2</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -1538,19 +1497,18 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+    <row r="40" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="1"/>
       <c r="C40" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D40" s="1">
         <v>3</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1558,21 +1516,18 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
+    <row r="41" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C41" s="2" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D41" s="1">
         <v>3</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -1580,19 +1535,18 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+    <row r="42" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="1"/>
       <c r="C42" s="2" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D42" s="1">
         <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -1600,19 +1554,18 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
+    <row r="43" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="1"/>
       <c r="C43" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D43" s="1">
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1620,19 +1573,18 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
+    <row r="44" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="1"/>
       <c r="C44" s="2" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="D44" s="1">
         <v>4</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -1640,19 +1592,18 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
+    <row r="45" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D45" s="1">
         <v>2</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -1660,19 +1611,18 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
+    <row r="46" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="1"/>
       <c r="C46" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D46" s="1">
         <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -1680,19 +1630,18 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
+    <row r="47" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="D47" s="1">
         <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -1700,19 +1649,18 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
+    <row r="48" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="D48" s="1">
         <v>3</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -1720,8 +1668,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
+    <row r="49" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1">

</xml_diff>